<commit_message>
add pdf sprint plan
</commit_message>
<xml_diff>
--- a/docs/sprint plan/Sprint plan 1.xlsx
+++ b/docs/sprint plan/Sprint plan 1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="37">
   <si>
     <t>User story</t>
   </si>
@@ -41,27 +41,9 @@
     <t>Sprint plan 1</t>
   </si>
   <si>
-    <t>context</t>
-  </si>
-  <si>
-    <t>Health Informatics</t>
-  </si>
-  <si>
-    <t>group</t>
-  </si>
-  <si>
     <t>product vision</t>
   </si>
   <si>
-    <t>Who is going to buy the product? Who is the target customer?</t>
-  </si>
-  <si>
-    <t>Which customer needs will the product address?</t>
-  </si>
-  <si>
-    <t>Which product attributes are crucial to satisfy the selected needs, and therefore to the succes of the product?</t>
-  </si>
-  <si>
     <t xml:space="preserve">As a user I want to generate an output file. </t>
   </si>
   <si>
@@ -147,6 +129,12 @@
   </si>
   <si>
     <t>software achitecture</t>
+  </si>
+  <si>
+    <t>group: 3</t>
+  </si>
+  <si>
+    <t>context: Health Informatics</t>
   </si>
 </sst>
 </file>
@@ -365,7 +353,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -376,25 +364,8 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
@@ -404,6 +375,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -684,18 +679,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="39.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.28515625" customWidth="1"/>
+    <col min="4" max="4" width="27.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -705,228 +700,205 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="2"/>
+    </row>
+    <row r="4" spans="1:4" s="23" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="22" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="19"/>
+      <c r="B6" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="19"/>
+      <c r="B7" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="18"/>
+      <c r="B8" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="19"/>
+      <c r="B10" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="18"/>
+      <c r="B11" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A4" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="10" t="s">
+      <c r="B12" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="18"/>
+      <c r="B13" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="19" t="s">
+      <c r="C13" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="D13" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="20"/>
+      <c r="B15" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
-      <c r="B6" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" s="4" t="s">
+      <c r="D19" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
-      <c r="B7" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="12"/>
-      <c r="B8" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" s="7" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="11"/>
-      <c r="B10" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="12"/>
-      <c r="B11" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="12"/>
-      <c r="B13" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
+      <c r="D20" t="s">
         <v>25</v>
-      </c>
-      <c r="B14" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="13"/>
-      <c r="B15" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B18" t="s">
-        <v>30</v>
-      </c>
-      <c r="D18" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B19" t="s">
-        <v>38</v>
-      </c>
-      <c r="D19" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B20" t="s">
-        <v>38</v>
-      </c>
-      <c r="D20" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G24" t="s">
-        <v>8</v>
-      </c>
-      <c r="H24" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H25" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H26" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -937,6 +909,6 @@
     <mergeCell ref="A5:A8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>